<commit_message>
add like and remove like method
</commit_message>
<xml_diff>
--- a/Blogging_DB design.xlsx
+++ b/Blogging_DB design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\blogging-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D630134E-1924-4B7B-BF0A-FBF3F34F27E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F664C9D-5075-4638-9A7A-05FFEEC147B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>TABLE NAME</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>Blog Image</t>
+  </si>
+  <si>
+    <t>[Array]</t>
+  </si>
+  <si>
+    <t>Liked user Id</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/blogs/addLike</t>
   </si>
 </sst>
 </file>
@@ -609,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -826,23 +838,29 @@
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
-      <c r="B12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
@@ -853,112 +871,126 @@
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="11" t="s">
-        <v>8</v>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
-      <c r="B19" s="10" t="s">
-        <v>36</v>
+      <c r="B19" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="11" t="s">
-        <v>8</v>
+        <v>36</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="8"/>
+      <c r="B21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" xr:uid="{50BEF9C1-7C82-4869-8B12-9E6A4D582236}"/>
     <hyperlink ref="F10" r:id="rId2" xr:uid="{8B629A11-7747-445F-99E4-80261E8E13C5}"/>
-    <hyperlink ref="F16" r:id="rId3" xr:uid="{694CF16D-6A8A-480C-BD07-5314CEC823C9}"/>
-    <hyperlink ref="F17" r:id="rId4" xr:uid="{C5DE05B0-AE7B-4A02-A2EB-57F81EB99D9A}"/>
+    <hyperlink ref="F17" r:id="rId3" xr:uid="{694CF16D-6A8A-480C-BD07-5314CEC823C9}"/>
+    <hyperlink ref="F18" r:id="rId4" xr:uid="{C5DE05B0-AE7B-4A02-A2EB-57F81EB99D9A}"/>
     <hyperlink ref="F11" r:id="rId5" xr:uid="{D04CA7D8-5A09-4CD5-9B5B-EFC624E7E768}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{0A7A6058-4DA9-4800-9926-67ED6EDF113A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>